<commit_message>
Cleaned up disciplinary actions for all 2016 WNYF home games
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-wnyf-crs-070116.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-wnyf-crs-070116.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/push/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1360" windowWidth="23520" windowHeight="12500" tabRatio="697"/>
+    <workbookView xWindow="-680" yWindow="460" windowWidth="22820" windowHeight="11180" tabRatio="697"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$AMK$1648</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$T$1648</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">match!$A$1:$T$1455</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">match!$A$1:$T$1455</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">match!$A$1:$T$1455</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16371" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16372" uniqueCount="236">
   <si>
     <t>event</t>
   </si>
@@ -1451,9 +1451,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1648"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1408" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1419" sqref="R1419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -67784,7 +67784,9 @@
       <c r="I1370" s="35"/>
       <c r="J1370" s="33"/>
       <c r="K1370" s="33"/>
-      <c r="L1370" s="36"/>
+      <c r="L1370" s="36" t="s">
+        <v>173</v>
+      </c>
       <c r="M1370" s="35"/>
       <c r="N1370" s="35"/>
       <c r="O1370" s="35"/>

</xml_diff>